<commit_message>
fixing code in data summary table
</commit_message>
<xml_diff>
--- a/Census_MainDB.xlsx
+++ b/Census_MainDB.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studugedu-my.sharepoint.com/personal/m_witkowska_ug_edu_pl/Documents/Dydaktyka/Ekologia zwierząt/Biologia/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studugedu-my.sharepoint.com/personal/m_witkowska_ug_edu_pl/Documents/Dydaktyka/Ekologia zwierząt/Animal-Ecology-Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="40" documentId="8_{E01B3394-57A6-4341-AD65-C10D062B73E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C8DE4C6E-9E82-432A-ADB5-A737313F80A1}"/>
+  <xr:revisionPtr revIDLastSave="138" documentId="8_{E01B3394-57A6-4341-AD65-C10D062B73E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BDE4A13-B519-435C-B887-F762B4FCBDB0}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{12B6839A-F7A1-4E86-8CA6-BC8CBCC96D2C}"/>
+    <workbookView xWindow="22932" yWindow="-4284" windowWidth="30936" windowHeight="17496" xr2:uid="{12B6839A-F7A1-4E86-8CA6-BC8CBCC96D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="3" r:id="rId1"/>
@@ -153,7 +153,7 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -183,6 +183,13 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -201,8 +208,9 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
   <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
@@ -213,8 +221,9 @@
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
+    <cellStyle name="Normalny 2" xfId="1" xr:uid="{AA74A43C-59BA-427E-8D7C-96F94B1ADD53}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -227,10 +236,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -532,17 +537,17 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DC50DC-4267-45C4-A865-09BFA7482B55}">
   <dimension ref="A1:I135"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A9" zoomScale="112" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="112" workbookViewId="0">
+      <selection activeCell="P138" sqref="P138"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="3" max="3" width="18.26953125" customWidth="1"/>
-    <col min="9" max="9" width="37.90625" customWidth="1"/>
+    <col min="3" max="3" width="18.21875" customWidth="1"/>
+    <col min="9" max="9" width="37.88671875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -569,7 +574,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -596,7 +601,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -623,7 +628,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -650,7 +655,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -677,7 +682,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -704,7 +709,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -731,7 +736,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -758,7 +763,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -785,7 +790,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -812,7 +817,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -839,7 +844,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -866,7 +871,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -893,7 +898,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -920,7 +925,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -947,7 +952,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -974,7 +979,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -1001,7 +1006,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -1028,7 +1033,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -1055,7 +1060,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -1082,7 +1087,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -1109,7 +1114,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -1136,7 +1141,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A23" s="2">
         <v>3</v>
       </c>
@@ -1163,7 +1168,7 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -1190,7 +1195,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -1217,7 +1222,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A26" s="2">
         <v>3</v>
       </c>
@@ -1244,7 +1249,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A27" s="2">
         <v>3</v>
       </c>
@@ -1271,7 +1276,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -1298,7 +1303,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A29" s="2">
         <v>3</v>
       </c>
@@ -1325,7 +1330,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -1352,7 +1357,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -1379,7 +1384,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A32" s="2">
         <v>3</v>
       </c>
@@ -1406,7 +1411,7 @@
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A33" s="2">
         <v>3</v>
       </c>
@@ -1433,7 +1438,7 @@
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A34" s="2">
         <v>3</v>
       </c>
@@ -1460,7 +1465,7 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -1487,7 +1492,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A36" s="2">
         <v>3</v>
       </c>
@@ -1514,7 +1519,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A37" s="2">
         <v>3</v>
       </c>
@@ -1541,7 +1546,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -1568,7 +1573,7 @@
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A39" s="2">
         <v>3</v>
       </c>
@@ -1595,7 +1600,7 @@
       </c>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A40" s="2">
         <v>3</v>
       </c>
@@ -1622,7 +1627,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -1649,7 +1654,7 @@
       </c>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A42" s="2">
         <v>3</v>
       </c>
@@ -1676,7 +1681,7 @@
       </c>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A43" s="2">
         <v>3</v>
       </c>
@@ -1703,7 +1708,7 @@
       </c>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A44" s="2">
         <v>3</v>
       </c>
@@ -1730,7 +1735,7 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -1757,7 +1762,7 @@
       </c>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A46" s="2">
         <v>3</v>
       </c>
@@ -1784,7 +1789,7 @@
       </c>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A47" s="2">
         <v>3</v>
       </c>
@@ -1811,7 +1816,7 @@
       </c>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A48" s="2">
         <v>3</v>
       </c>
@@ -1838,7 +1843,7 @@
       </c>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A49" s="2">
         <v>3</v>
       </c>
@@ -1865,7 +1870,7 @@
       </c>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A50" s="2">
         <v>2</v>
       </c>
@@ -1892,7 +1897,7 @@
       </c>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -1919,7 +1924,7 @@
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A52" s="2">
         <v>2</v>
       </c>
@@ -1946,7 +1951,7 @@
       </c>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A53" s="2">
         <v>2</v>
       </c>
@@ -1973,7 +1978,7 @@
       </c>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -2000,7 +2005,7 @@
       </c>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A55" s="2">
         <v>2</v>
       </c>
@@ -2027,7 +2032,7 @@
       </c>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A56" s="2">
         <v>2</v>
       </c>
@@ -2054,7 +2059,7 @@
       </c>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A57" s="2">
         <v>2</v>
       </c>
@@ -2081,7 +2086,7 @@
       </c>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A58" s="2">
         <v>2</v>
       </c>
@@ -2108,7 +2113,7 @@
       </c>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A59" s="2">
         <v>2</v>
       </c>
@@ -2135,7 +2140,7 @@
       </c>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A60" s="2">
         <v>2</v>
       </c>
@@ -2162,7 +2167,7 @@
       </c>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A61" s="2">
         <v>2</v>
       </c>
@@ -2189,7 +2194,7 @@
       </c>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A62" s="2">
         <v>2</v>
       </c>
@@ -2216,7 +2221,7 @@
       </c>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A63" s="2">
         <v>2</v>
       </c>
@@ -2243,7 +2248,7 @@
       </c>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A64" s="2">
         <v>2</v>
       </c>
@@ -2270,7 +2275,7 @@
       </c>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A65" s="2">
         <v>2</v>
       </c>
@@ -2297,7 +2302,7 @@
       </c>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A66" s="2">
         <v>2</v>
       </c>
@@ -2324,7 +2329,7 @@
       </c>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A67" s="2">
         <v>2</v>
       </c>
@@ -2351,7 +2356,7 @@
       </c>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A68" s="2">
         <v>2</v>
       </c>
@@ -2378,7 +2383,7 @@
       </c>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A69" s="2">
         <v>2</v>
       </c>
@@ -2405,7 +2410,7 @@
       </c>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A70" s="2">
         <v>2</v>
       </c>
@@ -2432,7 +2437,7 @@
       </c>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A71" s="2">
         <v>5</v>
       </c>
@@ -2459,7 +2464,7 @@
       </c>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A72" s="2">
         <v>5</v>
       </c>
@@ -2486,7 +2491,7 @@
       </c>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A73" s="2">
         <v>5</v>
       </c>
@@ -2513,7 +2518,7 @@
       </c>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A74" s="2">
         <v>5</v>
       </c>
@@ -2540,7 +2545,7 @@
       </c>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A75" s="2">
         <v>5</v>
       </c>
@@ -2567,7 +2572,7 @@
       </c>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A76" s="2">
         <v>5</v>
       </c>
@@ -2594,7 +2599,7 @@
       </c>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A77" s="2">
         <v>5</v>
       </c>
@@ -2621,7 +2626,7 @@
       </c>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A78" s="2">
         <v>5</v>
       </c>
@@ -2648,7 +2653,7 @@
       </c>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A79" s="2">
         <v>5</v>
       </c>
@@ -2675,7 +2680,7 @@
       </c>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A80" s="2">
         <v>5</v>
       </c>
@@ -2702,7 +2707,7 @@
       </c>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A81" s="2">
         <v>5</v>
       </c>
@@ -2729,7 +2734,7 @@
       </c>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A82" s="2">
         <v>5</v>
       </c>
@@ -2756,7 +2761,7 @@
       </c>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A83" s="2">
         <v>5</v>
       </c>
@@ -2783,7 +2788,7 @@
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A84" s="2">
         <v>5</v>
       </c>
@@ -2810,7 +2815,7 @@
       </c>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A85" s="2">
         <v>5</v>
       </c>
@@ -2837,7 +2842,7 @@
       </c>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A86" s="2">
         <v>5</v>
       </c>
@@ -2864,7 +2869,7 @@
       </c>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A87" s="2">
         <v>5</v>
       </c>
@@ -2891,7 +2896,7 @@
       </c>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A88" s="2">
         <v>5</v>
       </c>
@@ -2918,7 +2923,7 @@
       </c>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A89" s="2">
         <v>5</v>
       </c>
@@ -2945,7 +2950,7 @@
       </c>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A90" s="2">
         <v>5</v>
       </c>
@@ -2972,7 +2977,7 @@
       </c>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A91" s="2">
         <v>5</v>
       </c>
@@ -2999,7 +3004,7 @@
       </c>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A92" s="2">
         <v>5</v>
       </c>
@@ -3026,7 +3031,7 @@
       </c>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A93" s="2">
         <v>5</v>
       </c>
@@ -3053,7 +3058,7 @@
       </c>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A94" s="2">
         <v>5</v>
       </c>
@@ -3080,7 +3085,7 @@
       </c>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A95" s="2">
         <v>5</v>
       </c>
@@ -3107,7 +3112,7 @@
       </c>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A96" s="2">
         <v>5</v>
       </c>
@@ -3134,7 +3139,7 @@
       </c>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A97" s="2">
         <v>5</v>
       </c>
@@ -3161,7 +3166,7 @@
       </c>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A98" s="2">
         <v>5</v>
       </c>
@@ -3188,7 +3193,7 @@
       </c>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A99" s="2">
         <v>5</v>
       </c>
@@ -3215,7 +3220,7 @@
       </c>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A100" s="2">
         <v>5</v>
       </c>
@@ -3242,7 +3247,7 @@
       </c>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A101" s="2">
         <v>5</v>
       </c>
@@ -3269,7 +3274,7 @@
       </c>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A102" s="2">
         <v>5</v>
       </c>
@@ -3296,7 +3301,7 @@
       </c>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A103" s="2">
         <v>5</v>
       </c>
@@ -3323,7 +3328,7 @@
       </c>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A104" s="2">
         <v>5</v>
       </c>
@@ -3350,7 +3355,7 @@
       </c>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A105" s="2">
         <v>5</v>
       </c>
@@ -3377,7 +3382,7 @@
       </c>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A106" s="2">
         <v>5</v>
       </c>
@@ -3404,7 +3409,7 @@
       </c>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A107" s="2">
         <v>5</v>
       </c>
@@ -3431,7 +3436,7 @@
       </c>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A108" s="2">
         <v>5</v>
       </c>
@@ -3458,7 +3463,7 @@
       </c>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A109" s="2">
         <v>5</v>
       </c>
@@ -3485,7 +3490,7 @@
       </c>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A110" s="2">
         <v>5</v>
       </c>
@@ -3512,7 +3517,7 @@
       </c>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A111" s="2">
         <v>5</v>
       </c>
@@ -3539,7 +3544,7 @@
       </c>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A112" s="2">
         <v>5</v>
       </c>
@@ -3566,7 +3571,7 @@
       </c>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A113" s="2">
         <v>5</v>
       </c>
@@ -3593,7 +3598,7 @@
       </c>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A114" s="2">
         <v>5</v>
       </c>
@@ -3620,7 +3625,7 @@
       </c>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A115">
         <v>4</v>
       </c>
@@ -3647,7 +3652,7 @@
       </c>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A116">
         <v>4</v>
       </c>
@@ -3674,7 +3679,7 @@
       </c>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A117">
         <v>4</v>
       </c>
@@ -3701,7 +3706,7 @@
       </c>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A118">
         <v>4</v>
       </c>
@@ -3728,7 +3733,7 @@
       </c>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A119">
         <v>4</v>
       </c>
@@ -3755,7 +3760,7 @@
       </c>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A120">
         <v>4</v>
       </c>
@@ -3781,7 +3786,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A121">
         <v>4</v>
       </c>
@@ -3807,7 +3812,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A122">
         <v>4</v>
       </c>
@@ -3833,7 +3838,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A123">
         <v>4</v>
       </c>
@@ -3859,7 +3864,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A124">
         <v>4</v>
       </c>
@@ -3885,7 +3890,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A125">
         <v>4</v>
       </c>
@@ -3911,7 +3916,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A126">
         <v>4</v>
       </c>
@@ -3937,7 +3942,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A127">
         <v>4</v>
       </c>
@@ -3963,7 +3968,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.35">
+    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A128">
         <v>4</v>
       </c>
@@ -3989,7 +3994,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A129">
         <v>4</v>
       </c>
@@ -4015,7 +4020,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A130">
         <v>4</v>
       </c>
@@ -4041,7 +4046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A131">
         <v>4</v>
       </c>
@@ -4067,7 +4072,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A132">
         <v>4</v>
       </c>
@@ -4093,7 +4098,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A133">
         <v>4</v>
       </c>
@@ -4119,7 +4124,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A134">
         <v>4</v>
       </c>
@@ -4145,7 +4150,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
       <c r="A135">
         <v>4</v>
       </c>
@@ -4178,14 +4183,6 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1eaf5b92-17a7-4a6a-9207-70707233364f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Document" ma:contentTypeID="0x0101006DA9E7692837A34184F50E7C06ED0BEA" ma:contentTypeVersion="16" ma:contentTypeDescription="Create a new document." ma:contentTypeScope="" ma:versionID="873ae2f79fc2c8a8146ae12b21e75276">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns3="1eaf5b92-17a7-4a6a-9207-70707233364f" xmlns:ns4="b6d78ba6-cb2a-4ee1-831a-ac023f2ae066" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="03b39cda38b8052b54a8af630eafc1cc" ns3:_="" ns4:_="">
     <xsd:import namespace="1eaf5b92-17a7-4a6a-9207-70707233364f"/>
@@ -4426,6 +4423,14 @@
 </ct:contentTypeSchema>
 </file>
 
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1eaf5b92-17a7-4a6a-9207-70707233364f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
+</file>
+
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -4436,18 +4441,6 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79025B65-A6B6-4261-8E67-1795AEE1590C}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
-    <ds:schemaRef ds:uri="1eaf5b92-17a7-4a6a-9207-70707233364f"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{08CA95AE-F0AA-46BB-8726-212CF8FDC6C3}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -4467,6 +4460,18 @@
 </ds:datastoreItem>
 </file>
 
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79025B65-A6B6-4261-8E67-1795AEE1590C}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2000/xmlns/"/>
+    <ds:schemaRef ds:uri="1eaf5b92-17a7-4a6a-9207-70707233364f"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/2001/XMLSchema-instance"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E39A33D-06BE-4DAD-9367-E04591ABE29D}">
   <ds:schemaRefs>

</xml_diff>

<commit_message>
Updating data from students - census
</commit_message>
<xml_diff>
--- a/Census_MainDB.xlsx
+++ b/Census_MainDB.xlsx
@@ -1,22 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28129"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="28227"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://studugedu-my.sharepoint.com/personal/m_witkowska_ug_edu_pl/Documents/Dydaktyka/Ekologia zwierząt/Animal-Ecology-Lab/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="138" documentId="8_{E01B3394-57A6-4341-AD65-C10D062B73E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8BDE4A13-B519-435C-B887-F762B4FCBDB0}"/>
+  <xr:revisionPtr revIDLastSave="159" documentId="8_{E01B3394-57A6-4341-AD65-C10D062B73E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{C03D9A49-50A9-4CF0-8D48-02A0D7C65CEF}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-4284" windowWidth="30936" windowHeight="17496" xr2:uid="{12B6839A-F7A1-4E86-8CA6-BC8CBCC96D2C}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="25820" windowHeight="15500" xr2:uid="{12B6839A-F7A1-4E86-8CA6-BC8CBCC96D2C}"/>
   </bookViews>
   <sheets>
     <sheet name="Census" sheetId="3" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Census!$A$1:$I$135</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Census!$A$1:$I$258</definedName>
   </definedNames>
   <calcPr calcId="191028"/>
   <extLst>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="142" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="54">
   <si>
     <t>GRUPA</t>
   </si>
@@ -148,12 +148,66 @@
   <si>
     <t>gołąb</t>
   </si>
+  <si>
+    <t xml:space="preserve">kruk </t>
+  </si>
+  <si>
+    <t>mewa niezyidentyfikowana</t>
+  </si>
+  <si>
+    <t xml:space="preserve">modraszka </t>
+  </si>
+  <si>
+    <t xml:space="preserve">mewa srebrzysta </t>
+  </si>
+  <si>
+    <t>mewa śmieszka</t>
+  </si>
+  <si>
+    <t>gołąb skalny</t>
+  </si>
+  <si>
+    <t>kaczka krzyżówka</t>
+  </si>
+  <si>
+    <t>sikorka bogatka</t>
+  </si>
+  <si>
+    <t>dzięcioł</t>
+  </si>
+  <si>
+    <t>sosnówka</t>
+  </si>
+  <si>
+    <t>czapla siwa</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Łabędź niemy </t>
+  </si>
+  <si>
+    <t>raniuszek</t>
+  </si>
+  <si>
+    <t>paszkot</t>
+  </si>
+  <si>
+    <t>strzyżyk</t>
+  </si>
+  <si>
+    <t>mewa siwa</t>
+  </si>
+  <si>
+    <t>kowalik</t>
+  </si>
+  <si>
+    <t>mandarynka</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="9" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -190,6 +244,30 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <charset val="238"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Aptos"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF242424"/>
+      <name val="Aptos Narrow"/>
+      <charset val="1"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -212,7 +290,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="14">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
@@ -220,6 +298,27 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="right" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Normalny" xfId="0" builtinId="0"/>
@@ -535,19 +634,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{31DC50DC-4267-45C4-A865-09BFA7482B55}">
-  <dimension ref="A1:I135"/>
+  <sheetPr filterMode="1"/>
+  <dimension ref="A1:I258"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A69" zoomScale="112" workbookViewId="0">
-      <selection activeCell="P138" sqref="P138"/>
+    <sheetView tabSelected="1" zoomScale="112" workbookViewId="0">
+      <selection activeCell="I227" sqref="I227"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultColWidth="8.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="3" max="3" width="18.21875" customWidth="1"/>
-    <col min="9" max="9" width="37.88671875" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="9" max="9" width="37.90625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -574,7 +674,7 @@
       </c>
       <c r="I1" s="2"/>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A2" s="2">
         <v>3</v>
       </c>
@@ -601,7 +701,7 @@
       </c>
       <c r="I2" s="2"/>
     </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A3" s="2">
         <v>3</v>
       </c>
@@ -628,7 +728,7 @@
       </c>
       <c r="I3" s="2"/>
     </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A4" s="2">
         <v>3</v>
       </c>
@@ -655,7 +755,7 @@
       </c>
       <c r="I4" s="2"/>
     </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A5" s="2">
         <v>3</v>
       </c>
@@ -682,7 +782,7 @@
       </c>
       <c r="I5" s="2"/>
     </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A6" s="2">
         <v>3</v>
       </c>
@@ -709,7 +809,7 @@
       </c>
       <c r="I6" s="2"/>
     </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A7" s="2">
         <v>3</v>
       </c>
@@ -736,7 +836,7 @@
       </c>
       <c r="I7" s="2"/>
     </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A8" s="2">
         <v>3</v>
       </c>
@@ -763,7 +863,7 @@
       </c>
       <c r="I8" s="2"/>
     </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A9" s="2">
         <v>3</v>
       </c>
@@ -790,7 +890,7 @@
       </c>
       <c r="I9" s="2"/>
     </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A10" s="2">
         <v>3</v>
       </c>
@@ -817,7 +917,7 @@
       </c>
       <c r="I10" s="2"/>
     </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A11" s="2">
         <v>3</v>
       </c>
@@ -844,7 +944,7 @@
       </c>
       <c r="I11" s="2"/>
     </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A12" s="2">
         <v>3</v>
       </c>
@@ -871,7 +971,7 @@
       </c>
       <c r="I12" s="2"/>
     </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A13" s="2">
         <v>3</v>
       </c>
@@ -898,7 +998,7 @@
       </c>
       <c r="I13" s="2"/>
     </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A14" s="2">
         <v>3</v>
       </c>
@@ -925,7 +1025,7 @@
       </c>
       <c r="I14" s="2"/>
     </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A15" s="2">
         <v>3</v>
       </c>
@@ -952,7 +1052,7 @@
       </c>
       <c r="I15" s="2"/>
     </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A16" s="2">
         <v>3</v>
       </c>
@@ -979,7 +1079,7 @@
       </c>
       <c r="I16" s="2"/>
     </row>
-    <row r="17" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A17" s="2">
         <v>3</v>
       </c>
@@ -1006,7 +1106,7 @@
       </c>
       <c r="I17" s="2"/>
     </row>
-    <row r="18" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A18" s="2">
         <v>3</v>
       </c>
@@ -1033,7 +1133,7 @@
       </c>
       <c r="I18" s="2"/>
     </row>
-    <row r="19" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A19" s="2">
         <v>3</v>
       </c>
@@ -1060,7 +1160,7 @@
       </c>
       <c r="I19" s="2"/>
     </row>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A20" s="2">
         <v>3</v>
       </c>
@@ -1087,7 +1187,7 @@
       </c>
       <c r="I20" s="2"/>
     </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A21" s="2">
         <v>3</v>
       </c>
@@ -1114,7 +1214,7 @@
       </c>
       <c r="I21" s="2"/>
     </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A22" s="2">
         <v>3</v>
       </c>
@@ -1141,7 +1241,7 @@
       </c>
       <c r="I22" s="2"/>
     </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A23" s="2">
         <v>3</v>
       </c>
@@ -1168,7 +1268,7 @@
       </c>
       <c r="I23" s="2"/>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A24" s="2">
         <v>3</v>
       </c>
@@ -1195,7 +1295,7 @@
       </c>
       <c r="I24" s="2"/>
     </row>
-    <row r="25" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A25" s="2">
         <v>3</v>
       </c>
@@ -1222,7 +1322,7 @@
       </c>
       <c r="I25" s="2"/>
     </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A26" s="2">
         <v>3</v>
       </c>
@@ -1249,7 +1349,7 @@
       </c>
       <c r="I26" s="2"/>
     </row>
-    <row r="27" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A27" s="2">
         <v>3</v>
       </c>
@@ -1276,7 +1376,7 @@
       </c>
       <c r="I27" s="2"/>
     </row>
-    <row r="28" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A28" s="2">
         <v>3</v>
       </c>
@@ -1303,7 +1403,7 @@
       </c>
       <c r="I28" s="2"/>
     </row>
-    <row r="29" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A29" s="2">
         <v>3</v>
       </c>
@@ -1330,7 +1430,7 @@
       </c>
       <c r="I29" s="2"/>
     </row>
-    <row r="30" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A30" s="2">
         <v>3</v>
       </c>
@@ -1357,7 +1457,7 @@
       </c>
       <c r="I30" s="2"/>
     </row>
-    <row r="31" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A31" s="2">
         <v>3</v>
       </c>
@@ -1384,7 +1484,7 @@
       </c>
       <c r="I31" s="2"/>
     </row>
-    <row r="32" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A32" s="2">
         <v>3</v>
       </c>
@@ -1411,7 +1511,7 @@
       </c>
       <c r="I32" s="2"/>
     </row>
-    <row r="33" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A33" s="2">
         <v>3</v>
       </c>
@@ -1438,7 +1538,7 @@
       </c>
       <c r="I33" s="2"/>
     </row>
-    <row r="34" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A34" s="2">
         <v>3</v>
       </c>
@@ -1465,7 +1565,7 @@
       </c>
       <c r="I34" s="2"/>
     </row>
-    <row r="35" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A35" s="2">
         <v>3</v>
       </c>
@@ -1492,7 +1592,7 @@
       </c>
       <c r="I35" s="2"/>
     </row>
-    <row r="36" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A36" s="2">
         <v>3</v>
       </c>
@@ -1519,7 +1619,7 @@
       </c>
       <c r="I36" s="2"/>
     </row>
-    <row r="37" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A37" s="2">
         <v>3</v>
       </c>
@@ -1546,7 +1646,7 @@
       </c>
       <c r="I37" s="2"/>
     </row>
-    <row r="38" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A38" s="2">
         <v>3</v>
       </c>
@@ -1573,7 +1673,7 @@
       </c>
       <c r="I38" s="2"/>
     </row>
-    <row r="39" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A39" s="2">
         <v>3</v>
       </c>
@@ -1600,7 +1700,7 @@
       </c>
       <c r="I39" s="2"/>
     </row>
-    <row r="40" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A40" s="2">
         <v>3</v>
       </c>
@@ -1627,7 +1727,7 @@
       </c>
       <c r="I40" s="2"/>
     </row>
-    <row r="41" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A41" s="2">
         <v>3</v>
       </c>
@@ -1654,7 +1754,7 @@
       </c>
       <c r="I41" s="2"/>
     </row>
-    <row r="42" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A42" s="2">
         <v>3</v>
       </c>
@@ -1681,7 +1781,7 @@
       </c>
       <c r="I42" s="2"/>
     </row>
-    <row r="43" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A43" s="2">
         <v>3</v>
       </c>
@@ -1708,7 +1808,7 @@
       </c>
       <c r="I43" s="2"/>
     </row>
-    <row r="44" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A44" s="2">
         <v>3</v>
       </c>
@@ -1735,7 +1835,7 @@
       </c>
       <c r="I44" s="2"/>
     </row>
-    <row r="45" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A45" s="2">
         <v>3</v>
       </c>
@@ -1762,7 +1862,7 @@
       </c>
       <c r="I45" s="2"/>
     </row>
-    <row r="46" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="46" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A46" s="2">
         <v>3</v>
       </c>
@@ -1789,7 +1889,7 @@
       </c>
       <c r="I46" s="2"/>
     </row>
-    <row r="47" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="47" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A47" s="2">
         <v>3</v>
       </c>
@@ -1816,7 +1916,7 @@
       </c>
       <c r="I47" s="2"/>
     </row>
-    <row r="48" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="48" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A48" s="2">
         <v>3</v>
       </c>
@@ -1843,7 +1943,7 @@
       </c>
       <c r="I48" s="2"/>
     </row>
-    <row r="49" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="49" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A49" s="2">
         <v>3</v>
       </c>
@@ -1870,7 +1970,7 @@
       </c>
       <c r="I49" s="2"/>
     </row>
-    <row r="50" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="50" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A50" s="2">
         <v>2</v>
       </c>
@@ -1897,7 +1997,7 @@
       </c>
       <c r="I50" s="2"/>
     </row>
-    <row r="51" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="51" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A51" s="2">
         <v>2</v>
       </c>
@@ -1924,7 +2024,7 @@
       </c>
       <c r="I51" s="2"/>
     </row>
-    <row r="52" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="52" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A52" s="2">
         <v>2</v>
       </c>
@@ -1951,7 +2051,7 @@
       </c>
       <c r="I52" s="2"/>
     </row>
-    <row r="53" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="53" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A53" s="2">
         <v>2</v>
       </c>
@@ -1978,7 +2078,7 @@
       </c>
       <c r="I53" s="2"/>
     </row>
-    <row r="54" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="54" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A54" s="2">
         <v>2</v>
       </c>
@@ -2005,7 +2105,7 @@
       </c>
       <c r="I54" s="2"/>
     </row>
-    <row r="55" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="55" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A55" s="2">
         <v>2</v>
       </c>
@@ -2032,7 +2132,7 @@
       </c>
       <c r="I55" s="2"/>
     </row>
-    <row r="56" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="56" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A56" s="2">
         <v>2</v>
       </c>
@@ -2059,7 +2159,7 @@
       </c>
       <c r="I56" s="2"/>
     </row>
-    <row r="57" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="57" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A57" s="2">
         <v>2</v>
       </c>
@@ -2086,7 +2186,7 @@
       </c>
       <c r="I57" s="2"/>
     </row>
-    <row r="58" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="58" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A58" s="2">
         <v>2</v>
       </c>
@@ -2113,7 +2213,7 @@
       </c>
       <c r="I58" s="2"/>
     </row>
-    <row r="59" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="59" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A59" s="2">
         <v>2</v>
       </c>
@@ -2140,7 +2240,7 @@
       </c>
       <c r="I59" s="2"/>
     </row>
-    <row r="60" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="60" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A60" s="2">
         <v>2</v>
       </c>
@@ -2167,7 +2267,7 @@
       </c>
       <c r="I60" s="2"/>
     </row>
-    <row r="61" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="61" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A61" s="2">
         <v>2</v>
       </c>
@@ -2194,7 +2294,7 @@
       </c>
       <c r="I61" s="2"/>
     </row>
-    <row r="62" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="62" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A62" s="2">
         <v>2</v>
       </c>
@@ -2221,7 +2321,7 @@
       </c>
       <c r="I62" s="2"/>
     </row>
-    <row r="63" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="63" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A63" s="2">
         <v>2</v>
       </c>
@@ -2248,7 +2348,7 @@
       </c>
       <c r="I63" s="2"/>
     </row>
-    <row r="64" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="64" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A64" s="2">
         <v>2</v>
       </c>
@@ -2275,7 +2375,7 @@
       </c>
       <c r="I64" s="2"/>
     </row>
-    <row r="65" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="65" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A65" s="2">
         <v>2</v>
       </c>
@@ -2302,7 +2402,7 @@
       </c>
       <c r="I65" s="2"/>
     </row>
-    <row r="66" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="66" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A66" s="2">
         <v>2</v>
       </c>
@@ -2329,7 +2429,7 @@
       </c>
       <c r="I66" s="2"/>
     </row>
-    <row r="67" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="67" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A67" s="2">
         <v>2</v>
       </c>
@@ -2356,7 +2456,7 @@
       </c>
       <c r="I67" s="2"/>
     </row>
-    <row r="68" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="68" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A68" s="2">
         <v>2</v>
       </c>
@@ -2383,7 +2483,7 @@
       </c>
       <c r="I68" s="2"/>
     </row>
-    <row r="69" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="69" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A69" s="2">
         <v>2</v>
       </c>
@@ -2410,7 +2510,7 @@
       </c>
       <c r="I69" s="2"/>
     </row>
-    <row r="70" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="70" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A70" s="2">
         <v>2</v>
       </c>
@@ -2437,7 +2537,7 @@
       </c>
       <c r="I70" s="2"/>
     </row>
-    <row r="71" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="71" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A71" s="2">
         <v>5</v>
       </c>
@@ -2464,7 +2564,7 @@
       </c>
       <c r="I71" s="2"/>
     </row>
-    <row r="72" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="72" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A72" s="2">
         <v>5</v>
       </c>
@@ -2491,7 +2591,7 @@
       </c>
       <c r="I72" s="2"/>
     </row>
-    <row r="73" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="73" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A73" s="2">
         <v>5</v>
       </c>
@@ -2518,7 +2618,7 @@
       </c>
       <c r="I73" s="2"/>
     </row>
-    <row r="74" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="74" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A74" s="2">
         <v>5</v>
       </c>
@@ -2545,7 +2645,7 @@
       </c>
       <c r="I74" s="2"/>
     </row>
-    <row r="75" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="75" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A75" s="2">
         <v>5</v>
       </c>
@@ -2572,7 +2672,7 @@
       </c>
       <c r="I75" s="2"/>
     </row>
-    <row r="76" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="76" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A76" s="2">
         <v>5</v>
       </c>
@@ -2599,7 +2699,7 @@
       </c>
       <c r="I76" s="2"/>
     </row>
-    <row r="77" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="77" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A77" s="2">
         <v>5</v>
       </c>
@@ -2626,7 +2726,7 @@
       </c>
       <c r="I77" s="2"/>
     </row>
-    <row r="78" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="78" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A78" s="2">
         <v>5</v>
       </c>
@@ -2653,7 +2753,7 @@
       </c>
       <c r="I78" s="2"/>
     </row>
-    <row r="79" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="79" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A79" s="2">
         <v>5</v>
       </c>
@@ -2680,7 +2780,7 @@
       </c>
       <c r="I79" s="2"/>
     </row>
-    <row r="80" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="80" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A80" s="2">
         <v>5</v>
       </c>
@@ -2707,7 +2807,7 @@
       </c>
       <c r="I80" s="2"/>
     </row>
-    <row r="81" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="81" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A81" s="2">
         <v>5</v>
       </c>
@@ -2734,7 +2834,7 @@
       </c>
       <c r="I81" s="2"/>
     </row>
-    <row r="82" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="82" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A82" s="2">
         <v>5</v>
       </c>
@@ -2761,7 +2861,7 @@
       </c>
       <c r="I82" s="2"/>
     </row>
-    <row r="83" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="83" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A83" s="2">
         <v>5</v>
       </c>
@@ -2788,7 +2888,7 @@
       </c>
       <c r="I83" s="2"/>
     </row>
-    <row r="84" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="84" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A84" s="2">
         <v>5</v>
       </c>
@@ -2815,7 +2915,7 @@
       </c>
       <c r="I84" s="2"/>
     </row>
-    <row r="85" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="85" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A85" s="2">
         <v>5</v>
       </c>
@@ -2842,7 +2942,7 @@
       </c>
       <c r="I85" s="2"/>
     </row>
-    <row r="86" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="86" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A86" s="2">
         <v>5</v>
       </c>
@@ -2869,7 +2969,7 @@
       </c>
       <c r="I86" s="2"/>
     </row>
-    <row r="87" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="87" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A87" s="2">
         <v>5</v>
       </c>
@@ -2896,7 +2996,7 @@
       </c>
       <c r="I87" s="2"/>
     </row>
-    <row r="88" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="88" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A88" s="2">
         <v>5</v>
       </c>
@@ -2923,7 +3023,7 @@
       </c>
       <c r="I88" s="2"/>
     </row>
-    <row r="89" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="89" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A89" s="2">
         <v>5</v>
       </c>
@@ -2950,7 +3050,7 @@
       </c>
       <c r="I89" s="2"/>
     </row>
-    <row r="90" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="90" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A90" s="2">
         <v>5</v>
       </c>
@@ -2977,7 +3077,7 @@
       </c>
       <c r="I90" s="2"/>
     </row>
-    <row r="91" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="91" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A91" s="2">
         <v>5</v>
       </c>
@@ -3004,7 +3104,7 @@
       </c>
       <c r="I91" s="2"/>
     </row>
-    <row r="92" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="92" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A92" s="2">
         <v>5</v>
       </c>
@@ -3031,7 +3131,7 @@
       </c>
       <c r="I92" s="2"/>
     </row>
-    <row r="93" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="93" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A93" s="2">
         <v>5</v>
       </c>
@@ -3058,7 +3158,7 @@
       </c>
       <c r="I93" s="2"/>
     </row>
-    <row r="94" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="94" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A94" s="2">
         <v>5</v>
       </c>
@@ -3085,7 +3185,7 @@
       </c>
       <c r="I94" s="2"/>
     </row>
-    <row r="95" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="95" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A95" s="2">
         <v>5</v>
       </c>
@@ -3112,7 +3212,7 @@
       </c>
       <c r="I95" s="2"/>
     </row>
-    <row r="96" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="96" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A96" s="2">
         <v>5</v>
       </c>
@@ -3139,7 +3239,7 @@
       </c>
       <c r="I96" s="2"/>
     </row>
-    <row r="97" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="97" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A97" s="2">
         <v>5</v>
       </c>
@@ -3166,7 +3266,7 @@
       </c>
       <c r="I97" s="2"/>
     </row>
-    <row r="98" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="98" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A98" s="2">
         <v>5</v>
       </c>
@@ -3193,7 +3293,7 @@
       </c>
       <c r="I98" s="2"/>
     </row>
-    <row r="99" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="99" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A99" s="2">
         <v>5</v>
       </c>
@@ -3220,7 +3320,7 @@
       </c>
       <c r="I99" s="2"/>
     </row>
-    <row r="100" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="100" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A100" s="2">
         <v>5</v>
       </c>
@@ -3247,7 +3347,7 @@
       </c>
       <c r="I100" s="2"/>
     </row>
-    <row r="101" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="101" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A101" s="2">
         <v>5</v>
       </c>
@@ -3274,7 +3374,7 @@
       </c>
       <c r="I101" s="2"/>
     </row>
-    <row r="102" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="102" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A102" s="2">
         <v>5</v>
       </c>
@@ -3301,7 +3401,7 @@
       </c>
       <c r="I102" s="2"/>
     </row>
-    <row r="103" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="103" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A103" s="2">
         <v>5</v>
       </c>
@@ -3328,7 +3428,7 @@
       </c>
       <c r="I103" s="2"/>
     </row>
-    <row r="104" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="104" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A104" s="2">
         <v>5</v>
       </c>
@@ -3355,7 +3455,7 @@
       </c>
       <c r="I104" s="2"/>
     </row>
-    <row r="105" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="105" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A105" s="2">
         <v>5</v>
       </c>
@@ -3382,7 +3482,7 @@
       </c>
       <c r="I105" s="2"/>
     </row>
-    <row r="106" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="106" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A106" s="2">
         <v>5</v>
       </c>
@@ -3409,7 +3509,7 @@
       </c>
       <c r="I106" s="2"/>
     </row>
-    <row r="107" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="107" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A107" s="2">
         <v>5</v>
       </c>
@@ -3436,7 +3536,7 @@
       </c>
       <c r="I107" s="2"/>
     </row>
-    <row r="108" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="108" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A108" s="2">
         <v>5</v>
       </c>
@@ -3463,7 +3563,7 @@
       </c>
       <c r="I108" s="2"/>
     </row>
-    <row r="109" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="109" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A109" s="2">
         <v>5</v>
       </c>
@@ -3490,7 +3590,7 @@
       </c>
       <c r="I109" s="2"/>
     </row>
-    <row r="110" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="110" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A110" s="2">
         <v>5</v>
       </c>
@@ -3517,7 +3617,7 @@
       </c>
       <c r="I110" s="2"/>
     </row>
-    <row r="111" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="111" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A111" s="2">
         <v>5</v>
       </c>
@@ -3544,7 +3644,7 @@
       </c>
       <c r="I111" s="2"/>
     </row>
-    <row r="112" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="112" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A112" s="2">
         <v>5</v>
       </c>
@@ -3571,7 +3671,7 @@
       </c>
       <c r="I112" s="2"/>
     </row>
-    <row r="113" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="113" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A113" s="2">
         <v>5</v>
       </c>
@@ -3598,7 +3698,7 @@
       </c>
       <c r="I113" s="2"/>
     </row>
-    <row r="114" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="114" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A114" s="2">
         <v>5</v>
       </c>
@@ -3625,7 +3725,7 @@
       </c>
       <c r="I114" s="2"/>
     </row>
-    <row r="115" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="115" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A115">
         <v>4</v>
       </c>
@@ -3652,7 +3752,7 @@
       </c>
       <c r="I115" s="2"/>
     </row>
-    <row r="116" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="116" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A116">
         <v>4</v>
       </c>
@@ -3679,7 +3779,7 @@
       </c>
       <c r="I116" s="2"/>
     </row>
-    <row r="117" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="117" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A117">
         <v>4</v>
       </c>
@@ -3706,7 +3806,7 @@
       </c>
       <c r="I117" s="2"/>
     </row>
-    <row r="118" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="118" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A118">
         <v>4</v>
       </c>
@@ -3733,7 +3833,7 @@
       </c>
       <c r="I118" s="2"/>
     </row>
-    <row r="119" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="119" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A119">
         <v>4</v>
       </c>
@@ -3760,7 +3860,7 @@
       </c>
       <c r="I119" s="2"/>
     </row>
-    <row r="120" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="120" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A120">
         <v>4</v>
       </c>
@@ -3786,7 +3886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="121" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="121" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A121">
         <v>4</v>
       </c>
@@ -3812,7 +3912,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="122" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="122" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A122">
         <v>4</v>
       </c>
@@ -3838,7 +3938,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="123" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="123" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A123">
         <v>4</v>
       </c>
@@ -3864,7 +3964,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="124" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="124" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A124">
         <v>4</v>
       </c>
@@ -3890,7 +3990,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="125" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="125" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A125">
         <v>4</v>
       </c>
@@ -3916,7 +4016,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="126" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="126" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A126">
         <v>4</v>
       </c>
@@ -3942,7 +4042,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="127" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="127" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A127">
         <v>4</v>
       </c>
@@ -3968,7 +4068,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="128" spans="1:9" x14ac:dyDescent="0.3">
+    <row r="128" spans="1:9" hidden="1" x14ac:dyDescent="0.35">
       <c r="A128">
         <v>4</v>
       </c>
@@ -3994,7 +4094,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="129" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="129" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A129">
         <v>4</v>
       </c>
@@ -4020,7 +4120,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="130" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="130" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A130">
         <v>4</v>
       </c>
@@ -4046,7 +4146,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="131" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A131">
         <v>4</v>
       </c>
@@ -4072,7 +4172,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="132" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="132" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A132">
         <v>4</v>
       </c>
@@ -4098,7 +4198,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="133" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="133" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A133">
         <v>4</v>
       </c>
@@ -4124,7 +4224,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="134" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="134" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A134">
         <v>4</v>
       </c>
@@ -4150,7 +4250,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="135" spans="1:8" x14ac:dyDescent="0.3">
+    <row r="135" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
       <c r="A135">
         <v>4</v>
       </c>
@@ -4176,8 +4276,3212 @@
         <v>0</v>
       </c>
     </row>
+    <row r="136" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A136" s="5">
+        <v>1</v>
+      </c>
+      <c r="B136" s="5">
+        <v>1</v>
+      </c>
+      <c r="C136" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="D136" s="5">
+        <v>2</v>
+      </c>
+      <c r="E136" s="5">
+        <v>2</v>
+      </c>
+      <c r="F136" s="5">
+        <v>2</v>
+      </c>
+      <c r="G136" s="5">
+        <v>3</v>
+      </c>
+      <c r="H136" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="137" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A137" s="5">
+        <v>1</v>
+      </c>
+      <c r="B137" s="5">
+        <v>1</v>
+      </c>
+      <c r="C137" s="6" t="s">
+        <v>16</v>
+      </c>
+      <c r="D137" s="5">
+        <v>2</v>
+      </c>
+      <c r="E137" s="5">
+        <v>2</v>
+      </c>
+      <c r="F137" s="5">
+        <v>2</v>
+      </c>
+      <c r="G137" s="5">
+        <v>3</v>
+      </c>
+      <c r="H137" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="138" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A138" s="5">
+        <v>1</v>
+      </c>
+      <c r="B138" s="5">
+        <v>1</v>
+      </c>
+      <c r="C138" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D138" s="5">
+        <v>2</v>
+      </c>
+      <c r="E138" s="5">
+        <v>2</v>
+      </c>
+      <c r="F138" s="5">
+        <v>2</v>
+      </c>
+      <c r="G138" s="5">
+        <v>3</v>
+      </c>
+      <c r="H138" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="139" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A139" s="5">
+        <v>1</v>
+      </c>
+      <c r="B139" s="5">
+        <v>1</v>
+      </c>
+      <c r="C139" s="6" t="s">
+        <v>14</v>
+      </c>
+      <c r="D139" s="5">
+        <v>2</v>
+      </c>
+      <c r="E139" s="5">
+        <v>2</v>
+      </c>
+      <c r="F139" s="5">
+        <v>2</v>
+      </c>
+      <c r="G139" s="5">
+        <v>3</v>
+      </c>
+      <c r="H139" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="140" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A140" s="5">
+        <v>1</v>
+      </c>
+      <c r="B140" s="5">
+        <v>2</v>
+      </c>
+      <c r="C140" s="6" t="s">
+        <v>18</v>
+      </c>
+      <c r="D140" s="5">
+        <v>2</v>
+      </c>
+      <c r="E140" s="5">
+        <v>3</v>
+      </c>
+      <c r="F140" s="5">
+        <v>2</v>
+      </c>
+      <c r="G140" s="5">
+        <v>3</v>
+      </c>
+      <c r="H140" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="141" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A141" s="5">
+        <v>1</v>
+      </c>
+      <c r="B141" s="5">
+        <v>2</v>
+      </c>
+      <c r="C141" s="6" t="s">
+        <v>26</v>
+      </c>
+      <c r="D141" s="5">
+        <v>2</v>
+      </c>
+      <c r="E141" s="5">
+        <v>3</v>
+      </c>
+      <c r="F141" s="5">
+        <v>2</v>
+      </c>
+      <c r="G141" s="5">
+        <v>3</v>
+      </c>
+      <c r="H141" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="142" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A142">
+        <v>1</v>
+      </c>
+      <c r="B142">
+        <v>2</v>
+      </c>
+      <c r="C142" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D142">
+        <v>2</v>
+      </c>
+      <c r="E142">
+        <v>3</v>
+      </c>
+      <c r="F142">
+        <v>2</v>
+      </c>
+      <c r="G142" s="5">
+        <v>3</v>
+      </c>
+      <c r="H142">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="143" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A143">
+        <v>1</v>
+      </c>
+      <c r="B143">
+        <v>2</v>
+      </c>
+      <c r="C143" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D143">
+        <v>2</v>
+      </c>
+      <c r="E143">
+        <v>3</v>
+      </c>
+      <c r="F143">
+        <v>2</v>
+      </c>
+      <c r="G143" s="5">
+        <v>3</v>
+      </c>
+      <c r="H143">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="144" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A144">
+        <v>1</v>
+      </c>
+      <c r="B144">
+        <v>3</v>
+      </c>
+      <c r="C144" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D144">
+        <v>3</v>
+      </c>
+      <c r="E144">
+        <v>3</v>
+      </c>
+      <c r="F144">
+        <v>3</v>
+      </c>
+      <c r="G144">
+        <v>2</v>
+      </c>
+      <c r="H144">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="145" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A145">
+        <v>1</v>
+      </c>
+      <c r="B145">
+        <v>3</v>
+      </c>
+      <c r="C145" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="D145">
+        <v>3</v>
+      </c>
+      <c r="E145">
+        <v>3</v>
+      </c>
+      <c r="F145">
+        <v>3</v>
+      </c>
+      <c r="G145">
+        <v>2</v>
+      </c>
+      <c r="H145">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="146" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A146">
+        <v>1</v>
+      </c>
+      <c r="B146">
+        <v>4</v>
+      </c>
+      <c r="C146" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D146">
+        <v>3</v>
+      </c>
+      <c r="E146">
+        <v>3</v>
+      </c>
+      <c r="F146">
+        <v>2</v>
+      </c>
+      <c r="G146">
+        <v>2</v>
+      </c>
+      <c r="H146">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="147" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A147">
+        <v>1</v>
+      </c>
+      <c r="B147">
+        <v>4</v>
+      </c>
+      <c r="C147" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="D147">
+        <v>3</v>
+      </c>
+      <c r="E147">
+        <v>3</v>
+      </c>
+      <c r="F147">
+        <v>2</v>
+      </c>
+      <c r="G147">
+        <v>2</v>
+      </c>
+      <c r="H147">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="148" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A148">
+        <v>1</v>
+      </c>
+      <c r="B148">
+        <v>4</v>
+      </c>
+      <c r="C148" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="D148">
+        <v>3</v>
+      </c>
+      <c r="E148">
+        <v>3</v>
+      </c>
+      <c r="F148">
+        <v>2</v>
+      </c>
+      <c r="G148">
+        <v>2</v>
+      </c>
+      <c r="H148">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="149" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A149">
+        <v>1</v>
+      </c>
+      <c r="B149">
+        <v>5</v>
+      </c>
+      <c r="C149" s="7" t="s">
+        <v>26</v>
+      </c>
+      <c r="D149">
+        <v>3</v>
+      </c>
+      <c r="E149">
+        <v>1</v>
+      </c>
+      <c r="F149">
+        <v>3</v>
+      </c>
+      <c r="G149">
+        <v>2</v>
+      </c>
+      <c r="H149">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="150" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A150">
+        <v>1</v>
+      </c>
+      <c r="B150">
+        <v>5</v>
+      </c>
+      <c r="C150" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D150">
+        <v>3</v>
+      </c>
+      <c r="E150">
+        <v>1</v>
+      </c>
+      <c r="F150">
+        <v>3</v>
+      </c>
+      <c r="G150">
+        <v>2</v>
+      </c>
+      <c r="H150">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="151" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A151">
+        <v>1</v>
+      </c>
+      <c r="B151">
+        <v>5</v>
+      </c>
+      <c r="C151" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="D151">
+        <v>3</v>
+      </c>
+      <c r="E151">
+        <v>1</v>
+      </c>
+      <c r="F151">
+        <v>3</v>
+      </c>
+      <c r="G151">
+        <v>2</v>
+      </c>
+      <c r="H151">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="152" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A152">
+        <v>1</v>
+      </c>
+      <c r="B152">
+        <v>5</v>
+      </c>
+      <c r="C152" s="7" t="s">
+        <v>39</v>
+      </c>
+      <c r="D152">
+        <v>3</v>
+      </c>
+      <c r="E152">
+        <v>1</v>
+      </c>
+      <c r="F152">
+        <v>3</v>
+      </c>
+      <c r="G152">
+        <v>2</v>
+      </c>
+      <c r="H152">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="153" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A153">
+        <v>1</v>
+      </c>
+      <c r="B153">
+        <v>5</v>
+      </c>
+      <c r="C153" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D153">
+        <v>3</v>
+      </c>
+      <c r="E153">
+        <v>1</v>
+      </c>
+      <c r="F153">
+        <v>3</v>
+      </c>
+      <c r="G153">
+        <v>2</v>
+      </c>
+      <c r="H153">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="154" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A154">
+        <v>1</v>
+      </c>
+      <c r="B154">
+        <v>5</v>
+      </c>
+      <c r="C154" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D154">
+        <v>3</v>
+      </c>
+      <c r="E154">
+        <v>1</v>
+      </c>
+      <c r="F154">
+        <v>3</v>
+      </c>
+      <c r="G154">
+        <v>2</v>
+      </c>
+      <c r="H154">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="155" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A155">
+        <v>1</v>
+      </c>
+      <c r="B155">
+        <v>6</v>
+      </c>
+      <c r="C155" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="D155">
+        <v>2</v>
+      </c>
+      <c r="E155">
+        <v>3</v>
+      </c>
+      <c r="F155">
+        <v>2</v>
+      </c>
+      <c r="G155">
+        <v>2</v>
+      </c>
+      <c r="H155">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="156" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A156">
+        <v>1</v>
+      </c>
+      <c r="B156">
+        <v>6</v>
+      </c>
+      <c r="C156" s="7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D156">
+        <v>2</v>
+      </c>
+      <c r="E156">
+        <v>3</v>
+      </c>
+      <c r="F156">
+        <v>2</v>
+      </c>
+      <c r="G156">
+        <v>2</v>
+      </c>
+      <c r="H156">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="157" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A157">
+        <v>1</v>
+      </c>
+      <c r="B157">
+        <v>6</v>
+      </c>
+      <c r="C157" s="7" t="s">
+        <v>8</v>
+      </c>
+      <c r="D157">
+        <v>2</v>
+      </c>
+      <c r="E157">
+        <v>3</v>
+      </c>
+      <c r="F157">
+        <v>2</v>
+      </c>
+      <c r="G157">
+        <v>2</v>
+      </c>
+      <c r="H157">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="158" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A158">
+        <v>1</v>
+      </c>
+      <c r="B158">
+        <v>6</v>
+      </c>
+      <c r="C158" s="7" t="s">
+        <v>12</v>
+      </c>
+      <c r="D158">
+        <v>2</v>
+      </c>
+      <c r="E158">
+        <v>3</v>
+      </c>
+      <c r="F158">
+        <v>2</v>
+      </c>
+      <c r="G158">
+        <v>2</v>
+      </c>
+      <c r="H158">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="159" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A159">
+        <v>1</v>
+      </c>
+      <c r="B159">
+        <v>6</v>
+      </c>
+      <c r="C159" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="D159">
+        <v>2</v>
+      </c>
+      <c r="E159">
+        <v>3</v>
+      </c>
+      <c r="F159">
+        <v>2</v>
+      </c>
+      <c r="G159">
+        <v>2</v>
+      </c>
+      <c r="H159">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="160" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A160">
+        <v>1</v>
+      </c>
+      <c r="B160">
+        <v>6</v>
+      </c>
+      <c r="C160" s="7" t="s">
+        <v>40</v>
+      </c>
+      <c r="D160">
+        <v>2</v>
+      </c>
+      <c r="E160">
+        <v>3</v>
+      </c>
+      <c r="F160">
+        <v>2</v>
+      </c>
+      <c r="G160">
+        <v>2</v>
+      </c>
+      <c r="H160">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="161" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A161">
+        <v>5</v>
+      </c>
+      <c r="B161">
+        <v>1</v>
+      </c>
+      <c r="C161" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D161">
+        <v>2</v>
+      </c>
+      <c r="E161">
+        <v>1</v>
+      </c>
+      <c r="F161">
+        <v>1</v>
+      </c>
+      <c r="G161" s="5">
+        <v>3</v>
+      </c>
+      <c r="H161">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="162" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A162">
+        <v>5</v>
+      </c>
+      <c r="B162">
+        <v>1</v>
+      </c>
+      <c r="C162" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D162">
+        <v>2</v>
+      </c>
+      <c r="E162">
+        <v>1</v>
+      </c>
+      <c r="F162">
+        <v>1</v>
+      </c>
+      <c r="G162" s="5">
+        <v>3</v>
+      </c>
+      <c r="H162">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="163" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A163">
+        <v>5</v>
+      </c>
+      <c r="B163">
+        <v>1</v>
+      </c>
+      <c r="C163" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D163">
+        <v>2</v>
+      </c>
+      <c r="E163">
+        <v>1</v>
+      </c>
+      <c r="F163">
+        <v>1</v>
+      </c>
+      <c r="G163" s="5">
+        <v>3</v>
+      </c>
+      <c r="H163">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="164" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A164">
+        <v>5</v>
+      </c>
+      <c r="B164">
+        <v>1</v>
+      </c>
+      <c r="C164" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D164">
+        <v>2</v>
+      </c>
+      <c r="E164">
+        <v>1</v>
+      </c>
+      <c r="F164">
+        <v>1</v>
+      </c>
+      <c r="G164" s="5">
+        <v>3</v>
+      </c>
+      <c r="H164">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="165" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A165">
+        <v>5</v>
+      </c>
+      <c r="B165">
+        <v>1</v>
+      </c>
+      <c r="C165" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="D165">
+        <v>2</v>
+      </c>
+      <c r="E165">
+        <v>1</v>
+      </c>
+      <c r="F165">
+        <v>1</v>
+      </c>
+      <c r="G165" s="5">
+        <v>3</v>
+      </c>
+      <c r="H165">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="166" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A166">
+        <v>5</v>
+      </c>
+      <c r="B166">
+        <v>2</v>
+      </c>
+      <c r="C166" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D166">
+        <v>2</v>
+      </c>
+      <c r="E166">
+        <v>1</v>
+      </c>
+      <c r="F166">
+        <v>2</v>
+      </c>
+      <c r="G166">
+        <v>2</v>
+      </c>
+      <c r="H166">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="167" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A167">
+        <v>5</v>
+      </c>
+      <c r="B167">
+        <v>2</v>
+      </c>
+      <c r="C167" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D167">
+        <v>2</v>
+      </c>
+      <c r="E167">
+        <v>1</v>
+      </c>
+      <c r="F167">
+        <v>2</v>
+      </c>
+      <c r="G167">
+        <v>2</v>
+      </c>
+      <c r="H167">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="168" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A168">
+        <v>5</v>
+      </c>
+      <c r="B168">
+        <v>2</v>
+      </c>
+      <c r="C168" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D168">
+        <v>2</v>
+      </c>
+      <c r="E168">
+        <v>1</v>
+      </c>
+      <c r="F168">
+        <v>2</v>
+      </c>
+      <c r="G168">
+        <v>2</v>
+      </c>
+      <c r="H168">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="169" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A169">
+        <v>5</v>
+      </c>
+      <c r="B169">
+        <v>2</v>
+      </c>
+      <c r="C169" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D169">
+        <v>2</v>
+      </c>
+      <c r="E169">
+        <v>1</v>
+      </c>
+      <c r="F169">
+        <v>2</v>
+      </c>
+      <c r="G169">
+        <v>2</v>
+      </c>
+      <c r="H169">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="170" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A170">
+        <v>5</v>
+      </c>
+      <c r="B170">
+        <v>2</v>
+      </c>
+      <c r="C170" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D170">
+        <v>2</v>
+      </c>
+      <c r="E170">
+        <v>1</v>
+      </c>
+      <c r="F170">
+        <v>2</v>
+      </c>
+      <c r="G170">
+        <v>2</v>
+      </c>
+      <c r="H170">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="171" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A171">
+        <v>5</v>
+      </c>
+      <c r="B171">
+        <v>3</v>
+      </c>
+      <c r="C171" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D171">
+        <v>3</v>
+      </c>
+      <c r="E171">
+        <v>3</v>
+      </c>
+      <c r="F171">
+        <v>3</v>
+      </c>
+      <c r="G171">
+        <v>0</v>
+      </c>
+      <c r="H171">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="172" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A172">
+        <v>5</v>
+      </c>
+      <c r="B172">
+        <v>3</v>
+      </c>
+      <c r="C172" s="8" t="s">
+        <v>29</v>
+      </c>
+      <c r="D172">
+        <v>3</v>
+      </c>
+      <c r="E172">
+        <v>3</v>
+      </c>
+      <c r="F172">
+        <v>3</v>
+      </c>
+      <c r="G172">
+        <v>0</v>
+      </c>
+      <c r="H172">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="173" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A173">
+        <v>5</v>
+      </c>
+      <c r="B173">
+        <v>3</v>
+      </c>
+      <c r="C173" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D173">
+        <v>3</v>
+      </c>
+      <c r="E173">
+        <v>3</v>
+      </c>
+      <c r="F173">
+        <v>3</v>
+      </c>
+      <c r="G173">
+        <v>0</v>
+      </c>
+      <c r="H173">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="174" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A174">
+        <v>5</v>
+      </c>
+      <c r="B174">
+        <v>4</v>
+      </c>
+      <c r="C174" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D174">
+        <v>1</v>
+      </c>
+      <c r="E174">
+        <v>1</v>
+      </c>
+      <c r="F174">
+        <v>2</v>
+      </c>
+      <c r="G174">
+        <v>2</v>
+      </c>
+      <c r="H174">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="175" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A175">
+        <v>5</v>
+      </c>
+      <c r="B175">
+        <v>4</v>
+      </c>
+      <c r="C175" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D175">
+        <v>1</v>
+      </c>
+      <c r="E175">
+        <v>1</v>
+      </c>
+      <c r="F175">
+        <v>2</v>
+      </c>
+      <c r="G175">
+        <v>2</v>
+      </c>
+      <c r="H175">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="176" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A176">
+        <v>5</v>
+      </c>
+      <c r="B176">
+        <v>4</v>
+      </c>
+      <c r="C176" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="D176">
+        <v>1</v>
+      </c>
+      <c r="E176">
+        <v>1</v>
+      </c>
+      <c r="F176">
+        <v>2</v>
+      </c>
+      <c r="G176">
+        <v>2</v>
+      </c>
+      <c r="H176">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="177" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A177">
+        <v>5</v>
+      </c>
+      <c r="B177">
+        <v>4</v>
+      </c>
+      <c r="C177" s="8" t="s">
+        <v>25</v>
+      </c>
+      <c r="D177">
+        <v>1</v>
+      </c>
+      <c r="E177">
+        <v>1</v>
+      </c>
+      <c r="F177">
+        <v>2</v>
+      </c>
+      <c r="G177">
+        <v>2</v>
+      </c>
+      <c r="H177">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="178" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A178">
+        <v>5</v>
+      </c>
+      <c r="B178">
+        <v>4</v>
+      </c>
+      <c r="C178" s="8" t="s">
+        <v>14</v>
+      </c>
+      <c r="D178">
+        <v>1</v>
+      </c>
+      <c r="E178">
+        <v>1</v>
+      </c>
+      <c r="F178">
+        <v>2</v>
+      </c>
+      <c r="G178">
+        <v>2</v>
+      </c>
+      <c r="H178">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="179" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A179">
+        <v>5</v>
+      </c>
+      <c r="B179">
+        <v>4</v>
+      </c>
+      <c r="C179" s="8" t="s">
+        <v>32</v>
+      </c>
+      <c r="D179">
+        <v>1</v>
+      </c>
+      <c r="E179">
+        <v>1</v>
+      </c>
+      <c r="F179">
+        <v>2</v>
+      </c>
+      <c r="G179">
+        <v>2</v>
+      </c>
+      <c r="H179">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="180" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A180">
+        <v>5</v>
+      </c>
+      <c r="B180">
+        <v>4</v>
+      </c>
+      <c r="C180" s="8" t="s">
+        <v>44</v>
+      </c>
+      <c r="D180">
+        <v>1</v>
+      </c>
+      <c r="E180">
+        <v>1</v>
+      </c>
+      <c r="F180">
+        <v>2</v>
+      </c>
+      <c r="G180">
+        <v>2</v>
+      </c>
+      <c r="H180">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="181" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A181">
+        <v>5</v>
+      </c>
+      <c r="B181">
+        <v>5</v>
+      </c>
+      <c r="C181" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D181">
+        <v>2</v>
+      </c>
+      <c r="E181">
+        <v>2</v>
+      </c>
+      <c r="F181">
+        <v>2</v>
+      </c>
+      <c r="G181">
+        <v>2</v>
+      </c>
+      <c r="H181">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="182" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A182">
+        <v>5</v>
+      </c>
+      <c r="B182">
+        <v>5</v>
+      </c>
+      <c r="C182" s="8" t="s">
+        <v>16</v>
+      </c>
+      <c r="D182">
+        <v>2</v>
+      </c>
+      <c r="E182">
+        <v>2</v>
+      </c>
+      <c r="F182">
+        <v>2</v>
+      </c>
+      <c r="G182">
+        <v>2</v>
+      </c>
+      <c r="H182">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="183" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A183">
+        <v>5</v>
+      </c>
+      <c r="B183">
+        <v>5</v>
+      </c>
+      <c r="C183" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="D183">
+        <v>2</v>
+      </c>
+      <c r="E183">
+        <v>2</v>
+      </c>
+      <c r="F183">
+        <v>2</v>
+      </c>
+      <c r="G183">
+        <v>2</v>
+      </c>
+      <c r="H183">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="184" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A184">
+        <v>5</v>
+      </c>
+      <c r="B184">
+        <v>5</v>
+      </c>
+      <c r="C184" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="D184">
+        <v>2</v>
+      </c>
+      <c r="E184">
+        <v>2</v>
+      </c>
+      <c r="F184">
+        <v>2</v>
+      </c>
+      <c r="G184">
+        <v>2</v>
+      </c>
+      <c r="H184">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="185" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A185">
+        <v>5</v>
+      </c>
+      <c r="B185">
+        <v>6</v>
+      </c>
+      <c r="C185" s="8" t="s">
+        <v>43</v>
+      </c>
+      <c r="D185">
+        <v>1</v>
+      </c>
+      <c r="E185">
+        <v>1</v>
+      </c>
+      <c r="F185">
+        <v>1</v>
+      </c>
+      <c r="G185" s="5">
+        <v>3</v>
+      </c>
+      <c r="H185">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="186" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A186">
+        <v>5</v>
+      </c>
+      <c r="B186">
+        <v>6</v>
+      </c>
+      <c r="C186" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="D186">
+        <v>1</v>
+      </c>
+      <c r="E186">
+        <v>1</v>
+      </c>
+      <c r="F186">
+        <v>1</v>
+      </c>
+      <c r="G186" s="5">
+        <v>3</v>
+      </c>
+      <c r="H186">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="187" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A187">
+        <v>3</v>
+      </c>
+      <c r="B187">
+        <v>1</v>
+      </c>
+      <c r="C187" s="9" t="s">
+        <v>12</v>
+      </c>
+      <c r="D187">
+        <v>2</v>
+      </c>
+      <c r="E187">
+        <v>2</v>
+      </c>
+      <c r="F187">
+        <v>2</v>
+      </c>
+      <c r="G187" s="5">
+        <v>3</v>
+      </c>
+      <c r="H187">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="188" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A188">
+        <v>3</v>
+      </c>
+      <c r="B188">
+        <v>1</v>
+      </c>
+      <c r="C188" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D188" s="11">
+        <v>2</v>
+      </c>
+      <c r="E188" s="11">
+        <v>2</v>
+      </c>
+      <c r="F188" s="11">
+        <v>2</v>
+      </c>
+      <c r="G188" s="5">
+        <v>3</v>
+      </c>
+      <c r="H188" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="189" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A189">
+        <v>3</v>
+      </c>
+      <c r="B189">
+        <v>1</v>
+      </c>
+      <c r="C189" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D189">
+        <v>2</v>
+      </c>
+      <c r="E189">
+        <v>2</v>
+      </c>
+      <c r="F189">
+        <v>2</v>
+      </c>
+      <c r="G189" s="5">
+        <v>3</v>
+      </c>
+      <c r="H189">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="190" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A190">
+        <v>3</v>
+      </c>
+      <c r="B190">
+        <v>1</v>
+      </c>
+      <c r="C190" s="10" t="s">
+        <v>22</v>
+      </c>
+      <c r="D190" s="11">
+        <v>2</v>
+      </c>
+      <c r="E190" s="11">
+        <v>2</v>
+      </c>
+      <c r="F190" s="11">
+        <v>2</v>
+      </c>
+      <c r="G190" s="5">
+        <v>3</v>
+      </c>
+      <c r="H190" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="191" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A191">
+        <v>3</v>
+      </c>
+      <c r="B191">
+        <v>1</v>
+      </c>
+      <c r="C191" s="10" t="s">
+        <v>45</v>
+      </c>
+      <c r="D191">
+        <v>2</v>
+      </c>
+      <c r="E191">
+        <v>2</v>
+      </c>
+      <c r="F191">
+        <v>2</v>
+      </c>
+      <c r="G191" s="5">
+        <v>3</v>
+      </c>
+      <c r="H191">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="192" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A192">
+        <v>3</v>
+      </c>
+      <c r="B192">
+        <v>1</v>
+      </c>
+      <c r="C192" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D192" s="11">
+        <v>2</v>
+      </c>
+      <c r="E192" s="11">
+        <v>2</v>
+      </c>
+      <c r="F192" s="11">
+        <v>2</v>
+      </c>
+      <c r="G192" s="5">
+        <v>3</v>
+      </c>
+      <c r="H192" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="193" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A193">
+        <v>3</v>
+      </c>
+      <c r="B193">
+        <v>1</v>
+      </c>
+      <c r="C193" s="10" t="s">
+        <v>29</v>
+      </c>
+      <c r="D193">
+        <v>2</v>
+      </c>
+      <c r="E193">
+        <v>2</v>
+      </c>
+      <c r="F193">
+        <v>2</v>
+      </c>
+      <c r="G193" s="5">
+        <v>3</v>
+      </c>
+      <c r="H193">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="194" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A194">
+        <v>3</v>
+      </c>
+      <c r="B194">
+        <v>1</v>
+      </c>
+      <c r="C194" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D194" s="11">
+        <v>2</v>
+      </c>
+      <c r="E194" s="11">
+        <v>2</v>
+      </c>
+      <c r="F194" s="11">
+        <v>2</v>
+      </c>
+      <c r="G194" s="5">
+        <v>3</v>
+      </c>
+      <c r="H194" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="195" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A195">
+        <v>3</v>
+      </c>
+      <c r="B195">
+        <v>1</v>
+      </c>
+      <c r="C195" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D195" s="11">
+        <v>2</v>
+      </c>
+      <c r="E195" s="11">
+        <v>2</v>
+      </c>
+      <c r="F195" s="11">
+        <v>2</v>
+      </c>
+      <c r="G195" s="5">
+        <v>3</v>
+      </c>
+      <c r="H195" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="196" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A196">
+        <v>3</v>
+      </c>
+      <c r="B196">
+        <v>2</v>
+      </c>
+      <c r="C196" s="10" t="s">
+        <v>18</v>
+      </c>
+      <c r="D196" s="11">
+        <v>2</v>
+      </c>
+      <c r="E196" s="11">
+        <v>2</v>
+      </c>
+      <c r="F196" s="11">
+        <v>3</v>
+      </c>
+      <c r="G196" s="5">
+        <v>3</v>
+      </c>
+      <c r="H196" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="197" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A197">
+        <v>3</v>
+      </c>
+      <c r="B197">
+        <v>2</v>
+      </c>
+      <c r="C197" s="10" t="s">
+        <v>46</v>
+      </c>
+      <c r="D197" s="11">
+        <v>2</v>
+      </c>
+      <c r="E197" s="11">
+        <v>2</v>
+      </c>
+      <c r="F197" s="11">
+        <v>3</v>
+      </c>
+      <c r="G197" s="5">
+        <v>3</v>
+      </c>
+      <c r="H197" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="198" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A198">
+        <v>3</v>
+      </c>
+      <c r="B198">
+        <v>2</v>
+      </c>
+      <c r="C198" s="10" t="s">
+        <v>47</v>
+      </c>
+      <c r="D198" s="11">
+        <v>2</v>
+      </c>
+      <c r="E198" s="11">
+        <v>2</v>
+      </c>
+      <c r="F198" s="11">
+        <v>3</v>
+      </c>
+      <c r="G198" s="5">
+        <v>3</v>
+      </c>
+      <c r="H198" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="199" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A199">
+        <v>3</v>
+      </c>
+      <c r="B199">
+        <v>2</v>
+      </c>
+      <c r="C199" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D199" s="11">
+        <v>2</v>
+      </c>
+      <c r="E199" s="11">
+        <v>2</v>
+      </c>
+      <c r="F199" s="11">
+        <v>3</v>
+      </c>
+      <c r="G199" s="5">
+        <v>3</v>
+      </c>
+      <c r="H199" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="200" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A200">
+        <v>3</v>
+      </c>
+      <c r="B200">
+        <v>2</v>
+      </c>
+      <c r="C200" s="10" t="s">
+        <v>13</v>
+      </c>
+      <c r="D200" s="11">
+        <v>2</v>
+      </c>
+      <c r="E200" s="11">
+        <v>2</v>
+      </c>
+      <c r="F200" s="11">
+        <v>3</v>
+      </c>
+      <c r="G200" s="5">
+        <v>3</v>
+      </c>
+      <c r="H200" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="201" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A201">
+        <v>3</v>
+      </c>
+      <c r="B201">
+        <v>2</v>
+      </c>
+      <c r="C201" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D201" s="11">
+        <v>2</v>
+      </c>
+      <c r="E201" s="11">
+        <v>2</v>
+      </c>
+      <c r="F201" s="11">
+        <v>3</v>
+      </c>
+      <c r="G201" s="5">
+        <v>3</v>
+      </c>
+      <c r="H201" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="202" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A202">
+        <v>3</v>
+      </c>
+      <c r="B202">
+        <v>2</v>
+      </c>
+      <c r="C202" s="10" t="s">
+        <v>15</v>
+      </c>
+      <c r="D202" s="11">
+        <v>2</v>
+      </c>
+      <c r="E202" s="11">
+        <v>2</v>
+      </c>
+      <c r="F202" s="11">
+        <v>3</v>
+      </c>
+      <c r="G202" s="5">
+        <v>3</v>
+      </c>
+      <c r="H202" s="11">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="203" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A203">
+        <v>3</v>
+      </c>
+      <c r="B203">
+        <v>3</v>
+      </c>
+      <c r="C203" s="10" t="s">
+        <v>16</v>
+      </c>
+      <c r="D203" s="11">
+        <v>2</v>
+      </c>
+      <c r="E203" s="11">
+        <v>1</v>
+      </c>
+      <c r="F203" s="11">
+        <v>2</v>
+      </c>
+      <c r="G203" s="5">
+        <v>3</v>
+      </c>
+      <c r="H203" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="204" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A204">
+        <v>3</v>
+      </c>
+      <c r="B204">
+        <v>3</v>
+      </c>
+      <c r="C204" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D204" s="11">
+        <v>2</v>
+      </c>
+      <c r="E204" s="11">
+        <v>1</v>
+      </c>
+      <c r="F204" s="11">
+        <v>2</v>
+      </c>
+      <c r="G204" s="5">
+        <v>3</v>
+      </c>
+      <c r="H204" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="205" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A205">
+        <v>3</v>
+      </c>
+      <c r="B205">
+        <v>3</v>
+      </c>
+      <c r="C205" s="10" t="s">
+        <v>48</v>
+      </c>
+      <c r="D205" s="11">
+        <v>2</v>
+      </c>
+      <c r="E205" s="11">
+        <v>1</v>
+      </c>
+      <c r="F205" s="11">
+        <v>2</v>
+      </c>
+      <c r="G205" s="5">
+        <v>3</v>
+      </c>
+      <c r="H205" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="206" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A206">
+        <v>3</v>
+      </c>
+      <c r="B206">
+        <v>3</v>
+      </c>
+      <c r="C206" s="10" t="s">
+        <v>17</v>
+      </c>
+      <c r="D206" s="11">
+        <v>2</v>
+      </c>
+      <c r="E206" s="11">
+        <v>1</v>
+      </c>
+      <c r="F206" s="11">
+        <v>2</v>
+      </c>
+      <c r="G206" s="5">
+        <v>3</v>
+      </c>
+      <c r="H206" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="207" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A207">
+        <v>3</v>
+      </c>
+      <c r="B207">
+        <v>3</v>
+      </c>
+      <c r="C207" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D207" s="11">
+        <v>2</v>
+      </c>
+      <c r="E207" s="11">
+        <v>1</v>
+      </c>
+      <c r="F207" s="11">
+        <v>2</v>
+      </c>
+      <c r="G207" s="5">
+        <v>3</v>
+      </c>
+      <c r="H207" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="208" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A208">
+        <v>3</v>
+      </c>
+      <c r="B208">
+        <v>3</v>
+      </c>
+      <c r="C208" s="10" t="s">
+        <v>49</v>
+      </c>
+      <c r="D208" s="11">
+        <v>2</v>
+      </c>
+      <c r="E208" s="11">
+        <v>1</v>
+      </c>
+      <c r="F208" s="11">
+        <v>2</v>
+      </c>
+      <c r="G208" s="5">
+        <v>3</v>
+      </c>
+      <c r="H208" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="209" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A209">
+        <v>3</v>
+      </c>
+      <c r="B209">
+        <v>3</v>
+      </c>
+      <c r="C209" s="10" t="s">
+        <v>50</v>
+      </c>
+      <c r="D209" s="11">
+        <v>2</v>
+      </c>
+      <c r="E209" s="11">
+        <v>1</v>
+      </c>
+      <c r="F209" s="11">
+        <v>2</v>
+      </c>
+      <c r="G209" s="5">
+        <v>3</v>
+      </c>
+      <c r="H209" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="210" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A210">
+        <v>3</v>
+      </c>
+      <c r="B210">
+        <v>4</v>
+      </c>
+      <c r="C210" s="10" t="s">
+        <v>12</v>
+      </c>
+      <c r="D210" s="11">
+        <v>2</v>
+      </c>
+      <c r="E210" s="11">
+        <v>2</v>
+      </c>
+      <c r="F210" s="11">
+        <v>2</v>
+      </c>
+      <c r="G210">
+        <v>2</v>
+      </c>
+      <c r="H210" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="211" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A211">
+        <v>3</v>
+      </c>
+      <c r="B211">
+        <v>4</v>
+      </c>
+      <c r="C211" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D211" s="11">
+        <v>2</v>
+      </c>
+      <c r="E211" s="11">
+        <v>2</v>
+      </c>
+      <c r="F211" s="11">
+        <v>2</v>
+      </c>
+      <c r="G211">
+        <v>2</v>
+      </c>
+      <c r="H211" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="212" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A212">
+        <v>3</v>
+      </c>
+      <c r="B212">
+        <v>5</v>
+      </c>
+      <c r="C212" s="10" t="s">
+        <v>14</v>
+      </c>
+      <c r="D212" s="11">
+        <v>2</v>
+      </c>
+      <c r="E212" s="11">
+        <v>2</v>
+      </c>
+      <c r="F212" s="11">
+        <v>3</v>
+      </c>
+      <c r="G212">
+        <v>2</v>
+      </c>
+      <c r="H212" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="213" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A213">
+        <v>3</v>
+      </c>
+      <c r="B213">
+        <v>6</v>
+      </c>
+      <c r="C213" s="10" t="s">
+        <v>40</v>
+      </c>
+      <c r="D213" s="11">
+        <v>3</v>
+      </c>
+      <c r="E213" s="11">
+        <v>3</v>
+      </c>
+      <c r="F213" s="11">
+        <v>3</v>
+      </c>
+      <c r="G213">
+        <v>2</v>
+      </c>
+      <c r="H213" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="214" spans="1:8" hidden="1" x14ac:dyDescent="0.35">
+      <c r="A214">
+        <v>3</v>
+      </c>
+      <c r="B214">
+        <v>6</v>
+      </c>
+      <c r="C214" s="10" t="s">
+        <v>41</v>
+      </c>
+      <c r="D214" s="11">
+        <v>3</v>
+      </c>
+      <c r="E214" s="11">
+        <v>3</v>
+      </c>
+      <c r="F214" s="11">
+        <v>3</v>
+      </c>
+      <c r="G214">
+        <v>2</v>
+      </c>
+      <c r="H214" s="11">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="215" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A215" s="5">
+        <v>6</v>
+      </c>
+      <c r="B215" s="5">
+        <v>1</v>
+      </c>
+      <c r="C215" s="12" t="s">
+        <v>8</v>
+      </c>
+      <c r="D215" s="5">
+        <v>1</v>
+      </c>
+      <c r="E215" s="5">
+        <v>3</v>
+      </c>
+      <c r="F215" s="5">
+        <v>1</v>
+      </c>
+      <c r="G215" s="5">
+        <v>3</v>
+      </c>
+      <c r="H215" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="216" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A216" s="5">
+        <v>6</v>
+      </c>
+      <c r="B216" s="5">
+        <v>1</v>
+      </c>
+      <c r="C216" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D216" s="5">
+        <v>1</v>
+      </c>
+      <c r="E216" s="5">
+        <v>3</v>
+      </c>
+      <c r="F216" s="5">
+        <v>1</v>
+      </c>
+      <c r="G216" s="5">
+        <v>3</v>
+      </c>
+      <c r="H216" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="217" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A217" s="5">
+        <v>6</v>
+      </c>
+      <c r="B217" s="5">
+        <v>1</v>
+      </c>
+      <c r="C217" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D217" s="5">
+        <v>1</v>
+      </c>
+      <c r="E217" s="5">
+        <v>3</v>
+      </c>
+      <c r="F217" s="5">
+        <v>1</v>
+      </c>
+      <c r="G217" s="5">
+        <v>3</v>
+      </c>
+      <c r="H217" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="218" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A218" s="5">
+        <v>6</v>
+      </c>
+      <c r="B218" s="5">
+        <v>1</v>
+      </c>
+      <c r="C218" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D218" s="5">
+        <v>1</v>
+      </c>
+      <c r="E218" s="5">
+        <v>3</v>
+      </c>
+      <c r="F218" s="5">
+        <v>1</v>
+      </c>
+      <c r="G218" s="5">
+        <v>3</v>
+      </c>
+      <c r="H218" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="219" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A219" s="5">
+        <v>6</v>
+      </c>
+      <c r="B219" s="5">
+        <v>1</v>
+      </c>
+      <c r="C219" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D219" s="5">
+        <v>1</v>
+      </c>
+      <c r="E219" s="5">
+        <v>3</v>
+      </c>
+      <c r="F219" s="5">
+        <v>1</v>
+      </c>
+      <c r="G219" s="5">
+        <v>3</v>
+      </c>
+      <c r="H219" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="220" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A220" s="5">
+        <v>6</v>
+      </c>
+      <c r="B220" s="5">
+        <v>1</v>
+      </c>
+      <c r="C220" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D220" s="5">
+        <v>1</v>
+      </c>
+      <c r="E220" s="5">
+        <v>3</v>
+      </c>
+      <c r="F220" s="5">
+        <v>1</v>
+      </c>
+      <c r="G220" s="5">
+        <v>3</v>
+      </c>
+      <c r="H220" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="221" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A221" s="5">
+        <v>6</v>
+      </c>
+      <c r="B221" s="5">
+        <v>1</v>
+      </c>
+      <c r="C221" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D221" s="5">
+        <v>1</v>
+      </c>
+      <c r="E221" s="5">
+        <v>3</v>
+      </c>
+      <c r="F221" s="5">
+        <v>1</v>
+      </c>
+      <c r="G221" s="5">
+        <v>3</v>
+      </c>
+      <c r="H221" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="222" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A222" s="5">
+        <v>6</v>
+      </c>
+      <c r="B222" s="5">
+        <v>1</v>
+      </c>
+      <c r="C222" t="s">
+        <v>29</v>
+      </c>
+      <c r="D222" s="5">
+        <v>1</v>
+      </c>
+      <c r="E222" s="5">
+        <v>3</v>
+      </c>
+      <c r="F222" s="5">
+        <v>1</v>
+      </c>
+      <c r="G222" s="5">
+        <v>3</v>
+      </c>
+      <c r="H222" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="223" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A223" s="5">
+        <v>6</v>
+      </c>
+      <c r="B223">
+        <v>2</v>
+      </c>
+      <c r="C223" t="s">
+        <v>8</v>
+      </c>
+      <c r="D223" s="5">
+        <v>1</v>
+      </c>
+      <c r="E223" s="5">
+        <v>2</v>
+      </c>
+      <c r="F223" s="5">
+        <v>2</v>
+      </c>
+      <c r="G223" s="5">
+        <v>3</v>
+      </c>
+      <c r="H223" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="224" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A224" s="5">
+        <v>6</v>
+      </c>
+      <c r="B224">
+        <v>2</v>
+      </c>
+      <c r="C224" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D224" s="5">
+        <v>1</v>
+      </c>
+      <c r="E224" s="5">
+        <v>2</v>
+      </c>
+      <c r="F224" s="5">
+        <v>2</v>
+      </c>
+      <c r="G224" s="5">
+        <v>3</v>
+      </c>
+      <c r="H224" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="225" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A225" s="5">
+        <v>6</v>
+      </c>
+      <c r="B225">
+        <v>2</v>
+      </c>
+      <c r="C225" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D225" s="5">
+        <v>1</v>
+      </c>
+      <c r="E225" s="5">
+        <v>2</v>
+      </c>
+      <c r="F225" s="5">
+        <v>2</v>
+      </c>
+      <c r="G225" s="5">
+        <v>3</v>
+      </c>
+      <c r="H225" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="226" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A226" s="5">
+        <v>6</v>
+      </c>
+      <c r="B226">
+        <v>2</v>
+      </c>
+      <c r="C226" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D226" s="5">
+        <v>1</v>
+      </c>
+      <c r="E226" s="5">
+        <v>2</v>
+      </c>
+      <c r="F226" s="5">
+        <v>2</v>
+      </c>
+      <c r="G226" s="5">
+        <v>3</v>
+      </c>
+      <c r="H226" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="227" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A227" s="5">
+        <v>6</v>
+      </c>
+      <c r="B227">
+        <v>2</v>
+      </c>
+      <c r="C227" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D227" s="5">
+        <v>1</v>
+      </c>
+      <c r="E227" s="5">
+        <v>2</v>
+      </c>
+      <c r="F227" s="5">
+        <v>2</v>
+      </c>
+      <c r="G227" s="5">
+        <v>3</v>
+      </c>
+      <c r="H227" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="228" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A228" s="5">
+        <v>6</v>
+      </c>
+      <c r="B228">
+        <v>2</v>
+      </c>
+      <c r="C228" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D228" s="5">
+        <v>1</v>
+      </c>
+      <c r="E228" s="5">
+        <v>2</v>
+      </c>
+      <c r="F228" s="5">
+        <v>2</v>
+      </c>
+      <c r="G228" s="5">
+        <v>3</v>
+      </c>
+      <c r="H228" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="229" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A229" s="5">
+        <v>6</v>
+      </c>
+      <c r="B229">
+        <v>2</v>
+      </c>
+      <c r="C229" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D229" s="5">
+        <v>1</v>
+      </c>
+      <c r="E229" s="5">
+        <v>2</v>
+      </c>
+      <c r="F229" s="5">
+        <v>2</v>
+      </c>
+      <c r="G229" s="5">
+        <v>3</v>
+      </c>
+      <c r="H229" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="230" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A230" s="5">
+        <v>6</v>
+      </c>
+      <c r="B230">
+        <v>2</v>
+      </c>
+      <c r="C230" s="13" t="s">
+        <v>29</v>
+      </c>
+      <c r="D230" s="5">
+        <v>1</v>
+      </c>
+      <c r="E230" s="5">
+        <v>2</v>
+      </c>
+      <c r="F230" s="5">
+        <v>2</v>
+      </c>
+      <c r="G230" s="5">
+        <v>3</v>
+      </c>
+      <c r="H230" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="231" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A231" s="5">
+        <v>6</v>
+      </c>
+      <c r="B231">
+        <v>3</v>
+      </c>
+      <c r="C231" t="s">
+        <v>8</v>
+      </c>
+      <c r="D231" s="5">
+        <v>2</v>
+      </c>
+      <c r="E231" s="5">
+        <v>2</v>
+      </c>
+      <c r="F231" s="5">
+        <v>2</v>
+      </c>
+      <c r="G231" s="5">
+        <v>3</v>
+      </c>
+      <c r="H231" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="232" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A232" s="5">
+        <v>6</v>
+      </c>
+      <c r="B232">
+        <v>3</v>
+      </c>
+      <c r="C232" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D232" s="5">
+        <v>2</v>
+      </c>
+      <c r="E232" s="5">
+        <v>2</v>
+      </c>
+      <c r="F232" s="5">
+        <v>2</v>
+      </c>
+      <c r="G232" s="5">
+        <v>3</v>
+      </c>
+      <c r="H232" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="233" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A233" s="5">
+        <v>6</v>
+      </c>
+      <c r="B233">
+        <v>3</v>
+      </c>
+      <c r="C233" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D233" s="5">
+        <v>2</v>
+      </c>
+      <c r="E233" s="5">
+        <v>2</v>
+      </c>
+      <c r="F233" s="5">
+        <v>2</v>
+      </c>
+      <c r="G233" s="5">
+        <v>3</v>
+      </c>
+      <c r="H233" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="234" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A234" s="5">
+        <v>6</v>
+      </c>
+      <c r="B234">
+        <v>3</v>
+      </c>
+      <c r="C234" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D234" s="5">
+        <v>2</v>
+      </c>
+      <c r="E234" s="5">
+        <v>2</v>
+      </c>
+      <c r="F234" s="5">
+        <v>2</v>
+      </c>
+      <c r="G234" s="5">
+        <v>3</v>
+      </c>
+      <c r="H234" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="235" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A235" s="5">
+        <v>6</v>
+      </c>
+      <c r="B235">
+        <v>3</v>
+      </c>
+      <c r="C235" s="13" t="s">
+        <v>14</v>
+      </c>
+      <c r="D235" s="5">
+        <v>2</v>
+      </c>
+      <c r="E235" s="5">
+        <v>2</v>
+      </c>
+      <c r="F235" s="5">
+        <v>2</v>
+      </c>
+      <c r="G235" s="5">
+        <v>3</v>
+      </c>
+      <c r="H235" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="236" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A236" s="5">
+        <v>6</v>
+      </c>
+      <c r="B236">
+        <v>3</v>
+      </c>
+      <c r="C236" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D236" s="5">
+        <v>2</v>
+      </c>
+      <c r="E236" s="5">
+        <v>2</v>
+      </c>
+      <c r="F236" s="5">
+        <v>2</v>
+      </c>
+      <c r="G236" s="5">
+        <v>3</v>
+      </c>
+      <c r="H236" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="237" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A237" s="5">
+        <v>6</v>
+      </c>
+      <c r="B237">
+        <v>4</v>
+      </c>
+      <c r="C237" t="s">
+        <v>14</v>
+      </c>
+      <c r="D237" s="5">
+        <v>3</v>
+      </c>
+      <c r="E237" s="5">
+        <v>3</v>
+      </c>
+      <c r="F237" s="5">
+        <v>2</v>
+      </c>
+      <c r="G237">
+        <v>2</v>
+      </c>
+      <c r="H237" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="238" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A238" s="5">
+        <v>6</v>
+      </c>
+      <c r="B238">
+        <v>4</v>
+      </c>
+      <c r="C238" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D238" s="5">
+        <v>3</v>
+      </c>
+      <c r="E238" s="5">
+        <v>3</v>
+      </c>
+      <c r="F238" s="5">
+        <v>2</v>
+      </c>
+      <c r="G238">
+        <v>2</v>
+      </c>
+      <c r="H238" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="239" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A239" s="5">
+        <v>6</v>
+      </c>
+      <c r="B239">
+        <v>4</v>
+      </c>
+      <c r="C239" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D239" s="5">
+        <v>3</v>
+      </c>
+      <c r="E239" s="5">
+        <v>3</v>
+      </c>
+      <c r="F239" s="5">
+        <v>2</v>
+      </c>
+      <c r="G239">
+        <v>2</v>
+      </c>
+      <c r="H239" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="240" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A240" s="5">
+        <v>6</v>
+      </c>
+      <c r="B240">
+        <v>4</v>
+      </c>
+      <c r="C240" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D240" s="5">
+        <v>3</v>
+      </c>
+      <c r="E240" s="5">
+        <v>3</v>
+      </c>
+      <c r="F240" s="5">
+        <v>2</v>
+      </c>
+      <c r="G240">
+        <v>2</v>
+      </c>
+      <c r="H240" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="241" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A241" s="5">
+        <v>6</v>
+      </c>
+      <c r="B241">
+        <v>4</v>
+      </c>
+      <c r="C241" s="13" t="s">
+        <v>51</v>
+      </c>
+      <c r="D241" s="5">
+        <v>3</v>
+      </c>
+      <c r="E241" s="5">
+        <v>3</v>
+      </c>
+      <c r="F241" s="5">
+        <v>2</v>
+      </c>
+      <c r="G241">
+        <v>2</v>
+      </c>
+      <c r="H241" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="242" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A242" s="5">
+        <v>6</v>
+      </c>
+      <c r="B242">
+        <v>4</v>
+      </c>
+      <c r="C242" s="13" t="s">
+        <v>16</v>
+      </c>
+      <c r="D242" s="5">
+        <v>3</v>
+      </c>
+      <c r="E242" s="5">
+        <v>3</v>
+      </c>
+      <c r="F242" s="5">
+        <v>2</v>
+      </c>
+      <c r="G242">
+        <v>2</v>
+      </c>
+      <c r="H242" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="243" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A243" s="5">
+        <v>6</v>
+      </c>
+      <c r="B243">
+        <v>4</v>
+      </c>
+      <c r="C243" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D243" s="5">
+        <v>3</v>
+      </c>
+      <c r="E243" s="5">
+        <v>3</v>
+      </c>
+      <c r="F243" s="5">
+        <v>2</v>
+      </c>
+      <c r="G243">
+        <v>2</v>
+      </c>
+      <c r="H243" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="244" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A244" s="5">
+        <v>6</v>
+      </c>
+      <c r="B244">
+        <v>4</v>
+      </c>
+      <c r="C244" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D244" s="5">
+        <v>3</v>
+      </c>
+      <c r="E244" s="5">
+        <v>3</v>
+      </c>
+      <c r="F244" s="5">
+        <v>2</v>
+      </c>
+      <c r="G244">
+        <v>2</v>
+      </c>
+      <c r="H244" s="5">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="245" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A245" s="5">
+        <v>6</v>
+      </c>
+      <c r="B245">
+        <v>5</v>
+      </c>
+      <c r="C245" t="s">
+        <v>52</v>
+      </c>
+      <c r="D245" s="5">
+        <v>1</v>
+      </c>
+      <c r="E245" s="5">
+        <v>2</v>
+      </c>
+      <c r="F245" s="5">
+        <v>1</v>
+      </c>
+      <c r="G245" s="5">
+        <v>3</v>
+      </c>
+      <c r="H245" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="246" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A246" s="5">
+        <v>6</v>
+      </c>
+      <c r="B246">
+        <v>5</v>
+      </c>
+      <c r="C246" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D246" s="5">
+        <v>1</v>
+      </c>
+      <c r="E246" s="5">
+        <v>2</v>
+      </c>
+      <c r="F246" s="5">
+        <v>1</v>
+      </c>
+      <c r="G246" s="5">
+        <v>3</v>
+      </c>
+      <c r="H246" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="247" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A247" s="5">
+        <v>6</v>
+      </c>
+      <c r="B247">
+        <v>5</v>
+      </c>
+      <c r="C247" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D247" s="5">
+        <v>1</v>
+      </c>
+      <c r="E247" s="5">
+        <v>2</v>
+      </c>
+      <c r="F247" s="5">
+        <v>1</v>
+      </c>
+      <c r="G247" s="5">
+        <v>3</v>
+      </c>
+      <c r="H247" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="248" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A248" s="5">
+        <v>6</v>
+      </c>
+      <c r="B248">
+        <v>5</v>
+      </c>
+      <c r="C248" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D248" s="5">
+        <v>1</v>
+      </c>
+      <c r="E248" s="5">
+        <v>2</v>
+      </c>
+      <c r="F248" s="5">
+        <v>1</v>
+      </c>
+      <c r="G248" s="5">
+        <v>3</v>
+      </c>
+      <c r="H248" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="249" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A249" s="5">
+        <v>6</v>
+      </c>
+      <c r="B249">
+        <v>5</v>
+      </c>
+      <c r="C249" s="13" t="s">
+        <v>13</v>
+      </c>
+      <c r="D249" s="5">
+        <v>1</v>
+      </c>
+      <c r="E249" s="5">
+        <v>2</v>
+      </c>
+      <c r="F249" s="5">
+        <v>1</v>
+      </c>
+      <c r="G249" s="5">
+        <v>3</v>
+      </c>
+      <c r="H249" s="5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="250" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A250" s="5">
+        <v>6</v>
+      </c>
+      <c r="B250">
+        <v>6</v>
+      </c>
+      <c r="C250" t="s">
+        <v>29</v>
+      </c>
+      <c r="D250" s="5">
+        <v>1</v>
+      </c>
+      <c r="E250" s="5">
+        <v>1</v>
+      </c>
+      <c r="F250" s="5">
+        <v>2</v>
+      </c>
+      <c r="G250" s="5">
+        <v>3</v>
+      </c>
+      <c r="H250" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="251" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A251" s="5">
+        <v>6</v>
+      </c>
+      <c r="B251">
+        <v>6</v>
+      </c>
+      <c r="C251" s="13" t="s">
+        <v>8</v>
+      </c>
+      <c r="D251" s="5">
+        <v>1</v>
+      </c>
+      <c r="E251" s="5">
+        <v>1</v>
+      </c>
+      <c r="F251" s="5">
+        <v>2</v>
+      </c>
+      <c r="G251" s="5">
+        <v>3</v>
+      </c>
+      <c r="H251" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="252" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A252" s="5">
+        <v>6</v>
+      </c>
+      <c r="B252">
+        <v>6</v>
+      </c>
+      <c r="C252" s="13" t="s">
+        <v>18</v>
+      </c>
+      <c r="D252" s="5">
+        <v>1</v>
+      </c>
+      <c r="E252" s="5">
+        <v>1</v>
+      </c>
+      <c r="F252" s="5">
+        <v>2</v>
+      </c>
+      <c r="G252" s="5">
+        <v>3</v>
+      </c>
+      <c r="H252" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="253" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A253" s="5">
+        <v>6</v>
+      </c>
+      <c r="B253">
+        <v>6</v>
+      </c>
+      <c r="C253" s="13" t="s">
+        <v>53</v>
+      </c>
+      <c r="D253" s="5">
+        <v>1</v>
+      </c>
+      <c r="E253" s="5">
+        <v>1</v>
+      </c>
+      <c r="F253" s="5">
+        <v>2</v>
+      </c>
+      <c r="G253" s="5">
+        <v>3</v>
+      </c>
+      <c r="H253" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="254" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A254" s="5">
+        <v>6</v>
+      </c>
+      <c r="B254">
+        <v>6</v>
+      </c>
+      <c r="C254" s="13" t="s">
+        <v>26</v>
+      </c>
+      <c r="D254" s="5">
+        <v>1</v>
+      </c>
+      <c r="E254" s="5">
+        <v>1</v>
+      </c>
+      <c r="F254" s="5">
+        <v>2</v>
+      </c>
+      <c r="G254" s="5">
+        <v>3</v>
+      </c>
+      <c r="H254" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="255" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A255" s="5">
+        <v>6</v>
+      </c>
+      <c r="B255">
+        <v>6</v>
+      </c>
+      <c r="C255" s="13" t="s">
+        <v>15</v>
+      </c>
+      <c r="D255" s="5">
+        <v>1</v>
+      </c>
+      <c r="E255" s="5">
+        <v>1</v>
+      </c>
+      <c r="F255" s="5">
+        <v>2</v>
+      </c>
+      <c r="G255" s="5">
+        <v>3</v>
+      </c>
+      <c r="H255" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="256" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A256" s="5">
+        <v>6</v>
+      </c>
+      <c r="B256">
+        <v>6</v>
+      </c>
+      <c r="C256" s="13" t="s">
+        <v>12</v>
+      </c>
+      <c r="D256" s="5">
+        <v>1</v>
+      </c>
+      <c r="E256" s="5">
+        <v>1</v>
+      </c>
+      <c r="F256" s="5">
+        <v>2</v>
+      </c>
+      <c r="G256" s="5">
+        <v>3</v>
+      </c>
+      <c r="H256" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="257" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A257" s="5">
+        <v>6</v>
+      </c>
+      <c r="B257">
+        <v>6</v>
+      </c>
+      <c r="C257" s="13" t="s">
+        <v>9</v>
+      </c>
+      <c r="D257" s="5">
+        <v>1</v>
+      </c>
+      <c r="E257" s="5">
+        <v>1</v>
+      </c>
+      <c r="F257" s="5">
+        <v>2</v>
+      </c>
+      <c r="G257" s="5">
+        <v>3</v>
+      </c>
+      <c r="H257" s="5">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="258" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A258" s="5">
+        <v>6</v>
+      </c>
+      <c r="B258">
+        <v>6</v>
+      </c>
+      <c r="C258" s="13" t="s">
+        <v>10</v>
+      </c>
+      <c r="D258" s="5">
+        <v>1</v>
+      </c>
+      <c r="E258" s="5">
+        <v>1</v>
+      </c>
+      <c r="F258" s="5">
+        <v>2</v>
+      </c>
+      <c r="G258" s="5">
+        <v>3</v>
+      </c>
+      <c r="H258" s="5">
+        <v>3</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter ref="A1:I135" xr:uid="{31DC50DC-4267-45C4-A865-09BFA7482B55}"/>
+  <autoFilter ref="A1:I258" xr:uid="{31DC50DC-4267-45C4-A865-09BFA7482B55}">
+    <filterColumn colId="0">
+      <filters>
+        <filter val="6"/>
+      </filters>
+    </filterColumn>
+  </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -4424,20 +7728,20 @@
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <_activity xmlns="1eaf5b92-17a7-4a6a-9207-70707233364f" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
-</file>
-
-<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
   <Display>DocumentLibraryForm</Display>
   <Edit>DocumentLibraryForm</Edit>
   <New>DocumentLibraryForm</New>
 </FormTemplates>
+</file>
+
+<file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <_activity xmlns="1eaf5b92-17a7-4a6a-9207-70707233364f" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -4461,6 +7765,14 @@
 </file>
 
 <file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E39A33D-06BE-4DAD-9367-E04591ABE29D}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{79025B65-A6B6-4261-8E67-1795AEE1590C}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
@@ -4470,12 +7782,4 @@
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
-</file>
-
-<file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{9E39A33D-06BE-4DAD-9367-E04591ABE29D}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
 </file>
</xml_diff>